<commit_message>
Make custom traits formatting consistent with default traits
</commit_message>
<xml_diff>
--- a/inst/app/www/Custom_traits_formulas_example.xlsx
+++ b/inst/app/www/Custom_traits_formulas_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vf-lumc-home.lumcnet.prod.intern\lumc-home$\sgijze\MyDocs\glycodash\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgijze\Desktop\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AB5E23-B83C-4873-BA55-9EB18123DEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398E1764-9254-4B72-B43D-E626096A8ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22714" yWindow="-231" windowWidth="23040" windowHeight="13897" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1810" yWindow="-15860" windowWidth="25420" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,35 +25,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>IgGI</t>
-  </si>
-  <si>
-    <t>IgGII</t>
-  </si>
-  <si>
-    <t>IgGIV</t>
-  </si>
-  <si>
-    <t>first_trait = 0.5 * H4N4 + H5N4</t>
-  </si>
-  <si>
-    <t>second_trait = H4N4 + H5N4</t>
-  </si>
-  <si>
-    <t>third_trait = (H4N4F1 + H5N4F1) / H3N4F1</t>
-  </si>
-  <si>
-    <t>fourth_trait = H5N4F1S2 * H4N4F1S1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>IgGI_first_trait</t>
+  </si>
+  <si>
+    <t>0.5 * (IgGI1H4N4F1 + IgGI1H5N4F1)</t>
+  </si>
+  <si>
+    <t>second_trait</t>
+  </si>
+  <si>
+    <t>IgGI1H4N4F1S1 / (IgGI1H4N4F1 + IgGI1H4N5F1S1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,50 +369,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>